<commit_message>
Initial draft of ObservationDefinition - not yet tied into build
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk/build@2483 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/source/observationdefinition/Analysis.xlsx
+++ b/source/observationdefinition/Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="24915" windowHeight="13860"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="24915" windowHeight="13800"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
   <si>
     <t>LOINC</t>
   </si>
@@ -148,6 +148,36 @@
   </si>
   <si>
     <t>datatype</t>
+  </si>
+  <si>
+    <t>.code</t>
+  </si>
+  <si>
+    <t>.category</t>
+  </si>
+  <si>
+    <t>.alias</t>
+  </si>
+  <si>
+    <t>.mapping</t>
+  </si>
+  <si>
+    <t>.name</t>
+  </si>
+  <si>
+    <t>.status</t>
+  </si>
+  <si>
+    <t>.question</t>
+  </si>
+  <si>
+    <t>.comments</t>
+  </si>
+  <si>
+    <t>.binding.reference</t>
+  </si>
+  <si>
+    <t>(how is this different from alias?)</t>
   </si>
 </sst>
 </file>
@@ -486,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +529,7 @@
     <col min="3" max="3" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -510,15 +540,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -526,55 +559,73 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -582,30 +633,39 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -613,42 +673,51 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -656,25 +725,31 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -682,12 +757,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>

</xml_diff>